<commit_message>
Final changes for releasing victor calls.
</commit_message>
<xml_diff>
--- a/AngularJSAuthentication.API/UploadFile/Leads.xlsx
+++ b/AngularJSAuthentication.API/UploadFile/Leads.xlsx
@@ -15,12 +15,11 @@
     <definedName name="Name">Sheet1!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -40,67 +39,22 @@
     <t>test@test.com</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "projectID": 1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "name": "Brochure",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 2,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/2"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 3,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "name": "Project.cs",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/3"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 4,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/4"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 5,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/5"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "documentID": 6,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "name": "CreateLeads Procedure.txt",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        "link": "http://api.victorcalls.com/api/Project/1/Document/6"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    }</t>
-  </si>
-  <si>
-    <t>]</t>
+    <t>Gagan</t>
+  </si>
+  <si>
+    <t>g@gagan.com</t>
+  </si>
+  <si>
+    <t>3 bhk</t>
+  </si>
+  <si>
+    <t>Himanshu</t>
+  </si>
+  <si>
+    <t>h@gmail.com</t>
+  </si>
+  <si>
+    <t>2bhk</t>
   </si>
 </sst>
 </file>
@@ -147,9 +101,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,240 +400,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2">
+        <v>9818786514</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>9818786514</v>
-      </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="G9" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="1">
+        <v>9876543212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="G12" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="G13" t="s">
+      <c r="B4" s="1">
+        <v>7849495611</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="G14" t="s">
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="G16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7">
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7">
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7">
-      <c r="G23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7">
-      <c r="G24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7">
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7">
-      <c r="G26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7">
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="7:7">
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7">
-      <c r="G29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="7:7">
-      <c r="G30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="7:7">
-      <c r="G31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="7:7">
-      <c r="G32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7">
-      <c r="G33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7">
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7">
-      <c r="G35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="7:7">
-      <c r="G36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7">
-      <c r="G37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="7:7">
-      <c r="G38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="7:7">
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7">
-      <c r="G40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="7:7">
-      <c r="G41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="7:7">
-      <c r="G42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="7:7">
-      <c r="G43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="7:7">
-      <c r="G44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="7:7">
-      <c r="G45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="7:7">
-      <c r="G46" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>